<commit_message>
regimen added + eye level fix
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.3.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,6 +30,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'block new'!$A$1:$K$116</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">main!$A$1:$F$308</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$288</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$308</definedName>
@@ -57,6 +58,7 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$460</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$460</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$460</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$460</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4265" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="215">
   <si>
     <t>kpi Name</t>
   </si>
@@ -560,6 +562,12 @@
   </si>
   <si>
     <t>sud_orchestration</t>
+  </si>
+  <si>
+    <t>Blocking:Regimen_Presence:FABRIC_CARE</t>
+  </si>
+  <si>
+    <t>fabricare_regimen</t>
   </si>
   <si>
     <t>brand_list</t>
@@ -1100,7 +1108,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A469 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1195,14 +1203,14 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="A469 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.9514170040486"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
@@ -1225,7 +1233,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,7 +1420,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="1" sqref="A469 E28"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,7 +1439,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>19</v>
@@ -1451,13 +1459,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>38</v>
@@ -1471,13 +1479,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>38</v>
@@ -1502,7 +1510,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="A469 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1515,22 +1523,22 @@
         <v>16</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,13 +1549,13 @@
         <v>21</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>38</v>
@@ -1561,19 +1569,19 @@
         <v>21</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,13 +1592,13 @@
         <v>21</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>38</v>
@@ -1604,13 +1612,13 @@
         <v>21</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>38</v>
@@ -1627,13 +1635,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,13 +1652,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1680,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A469 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1691,7 +1699,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>19</v>
@@ -1711,13 +1719,13 @@
         <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1739,12 +1747,12 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A469 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7408906882591"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1753,52 +1761,52 @@
         <v>16</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Q1" s="27" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,37 +1817,37 @@
         <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>202</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>1</v>
@@ -1856,14 +1864,14 @@
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D3" s="28"/>
       <c r="H3" s="28" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="N3" s="28" t="n">
         <v>1</v>
@@ -1880,13 +1888,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
@@ -1912,10 +1920,10 @@
         <v>7</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
@@ -1949,7 +1957,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="A469 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2008,7 +2016,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="A469 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2415,12 +2423,12 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B62" activeCellId="1" sqref="A469 B62"/>
+      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="110.105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="111.080971659919"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3389,7 +3397,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A81" activeCellId="1" sqref="A469 A81"/>
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4483,17 +4491,17 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A109" activeCellId="1" sqref="A469 A109"/>
+      <selection pane="topLeft" activeCell="C123" activeCellId="0" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.0566801619433"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.7004048582996"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.67611336032389"/>
@@ -6606,7 +6614,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="1" sqref="A469 B11"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6881,16 +6889,16 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="1" sqref="A469 G37"/>
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -7600,13 +7608,13 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="1" sqref="A469 A23"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
@@ -8167,20 +8175,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F469"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A445" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A469" activeCellId="0" sqref="A469"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A435" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E470" activeCellId="0" sqref="E470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="90.7287449392713"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.7327935222672"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.587044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.4817813765182"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -16158,6 +16166,23 @@
       </c>
       <c r="E469" s="11" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C470" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D470" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E470" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>